<commit_message>
Added new sample queries
</commit_message>
<xml_diff>
--- a/P&P (2018) analysis/Source/P&P (2018) - Annex 2 - Data set.xlsx
+++ b/P&P (2018) analysis/Source/P&P (2018) - Annex 2 - Data set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\P&amp;P (2018) analysis\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0991D6-1241-4ABB-992E-CA902D011396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4489F7-1702-4FF1-A2D9-43FF86EF19E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1774,6 +1774,8 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1807,8 +1809,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2149,9 +2149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T1128" sqref="T1128"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2243,75 +2241,75 @@
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="74" t="s">
+      <c r="D6" s="76" t="s">
         <v>336</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="77" t="s">
         <v>337</v>
       </c>
-      <c r="F6" s="71" t="s">
+      <c r="F6" s="73" t="s">
         <v>343</v>
       </c>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71" t="s">
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73" t="s">
         <v>344</v>
       </c>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="71" t="s">
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73" t="s">
         <v>343</v>
       </c>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
       <c r="T6" s="31"/>
       <c r="U6" s="31"/>
       <c r="V6" s="31"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="82"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="76" t="s">
+      <c r="A7" s="71"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78" t="s">
         <v>338</v>
       </c>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="77" t="s">
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="K7" s="78"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="80" t="s">
+      <c r="K7" s="80"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="82" t="s">
         <v>339</v>
       </c>
-      <c r="N7" s="80"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="72" t="s">
+      <c r="N7" s="82"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="74" t="s">
         <v>330</v>
       </c>
-      <c r="Q7" s="72"/>
-      <c r="R7" s="73" t="s">
+      <c r="Q7" s="74"/>
+      <c r="R7" s="75" t="s">
         <v>331</v>
       </c>
-      <c r="S7" s="73"/>
+      <c r="S7" s="75"/>
       <c r="T7" s="31" t="s">
         <v>3</v>
       </c>
@@ -2319,12 +2317,12 @@
       <c r="V7" s="31"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="82"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="76"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="78"/>
       <c r="G8" s="32" t="s">
         <v>340</v>
       </c>
@@ -45589,11 +45587,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:O6"/>
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="R7:S7"/>
@@ -45603,6 +45596,11 @@
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="M7:O7"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:O6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>